<commit_message>
Ajustes geração de melhor rota e incluída novas cidades
</commit_message>
<xml_diff>
--- a/Coordenadas.xlsx
+++ b/Coordenadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igort\Documents\CaixeiroViajante\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB3D19A-06AC-4626-B5AA-95F2020F3A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A105EF5-0FA1-4826-866A-406A50F0F669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D42C705A-2AC4-45D4-A84C-5D4BDD70EA94}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D42C705A-2AC4-45D4-A84C-5D4BDD70EA94}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>São Paulo</t>
   </si>
@@ -126,6 +126,69 @@
   </si>
   <si>
     <t>-62,2159</t>
+  </si>
+  <si>
+    <t>Joinville</t>
+  </si>
+  <si>
+    <t>-26,3045</t>
+  </si>
+  <si>
+    <t>-48,8458</t>
+  </si>
+  <si>
+    <t>Lages</t>
+  </si>
+  <si>
+    <t>-27,815</t>
+  </si>
+  <si>
+    <t>-50,3259</t>
+  </si>
+  <si>
+    <t>Ouro Preto</t>
+  </si>
+  <si>
+    <t>-43,5031</t>
+  </si>
+  <si>
+    <t>Blumenal</t>
+  </si>
+  <si>
+    <t>-26,9195</t>
+  </si>
+  <si>
+    <t>-20,3856</t>
+  </si>
+  <si>
+    <t>-49,066</t>
+  </si>
+  <si>
+    <t>Florianopolis</t>
+  </si>
+  <si>
+    <t>-27,5949</t>
+  </si>
+  <si>
+    <t>-48,5482</t>
+  </si>
+  <si>
+    <t>Acre</t>
+  </si>
+  <si>
+    <t>-9,0238</t>
+  </si>
+  <si>
+    <t>-70,812</t>
+  </si>
+  <si>
+    <t>Fernando de Noronha</t>
+  </si>
+  <si>
+    <t>-3,8402</t>
+  </si>
+  <si>
+    <t>-32,4141</t>
   </si>
 </sst>
 </file>
@@ -182,7 +245,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,19 +560,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D66C6FB-D3EA-4E09-AF02-5C5E3F149BEC}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -520,7 +583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -531,7 +594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -542,7 +605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -563,8 +626,9 @@
       <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -575,7 +639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -586,7 +650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -597,7 +661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -608,7 +672,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -619,6 +683,86 @@
         <v>29</v>
       </c>
       <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>